<commit_message>
NLP Text  Bag of words
</commit_message>
<xml_diff>
--- a/Sales Prediction /Book01.xlsx
+++ b/Sales Prediction /Book01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asadtariq/Downloads/Python_work/Python_work/Sales Prediction /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3552F548-29D6-5B43-87B5-654A94CE4BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E574E0-1401-5A41-B6CE-81D6C9A92123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{FD4F2EBA-A1A6-448A-A246-9B6F55674063}"/>
   </bookViews>
@@ -422,11 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7DFC0D-7099-4BD6-B583-485D9FE3FFF5}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E500"/>
+  <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E504" sqref="E504"/>
+    <sheetView tabSelected="1" topLeftCell="A479" workbookViewId="0">
+      <selection activeCell="E501" sqref="E501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -453,7 +452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44197</v>
       </c>
@@ -470,7 +469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44198</v>
       </c>
@@ -487,7 +486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44199</v>
       </c>
@@ -504,7 +503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44200</v>
       </c>
@@ -521,7 +520,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -538,7 +537,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -555,7 +554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44203</v>
       </c>
@@ -572,7 +571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44204</v>
       </c>
@@ -589,7 +588,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44205</v>
       </c>
@@ -606,7 +605,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44206</v>
       </c>
@@ -623,7 +622,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44207</v>
       </c>
@@ -640,7 +639,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44208</v>
       </c>
@@ -657,7 +656,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44209</v>
       </c>
@@ -674,7 +673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44210</v>
       </c>
@@ -691,7 +690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44211</v>
       </c>
@@ -708,7 +707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44212</v>
       </c>
@@ -725,7 +724,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44213</v>
       </c>
@@ -742,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44214</v>
       </c>
@@ -759,7 +758,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44215</v>
       </c>
@@ -776,7 +775,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44216</v>
       </c>
@@ -793,7 +792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44217</v>
       </c>
@@ -810,7 +809,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44218</v>
       </c>
@@ -827,7 +826,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44219</v>
       </c>
@@ -844,7 +843,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44220</v>
       </c>
@@ -861,7 +860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44221</v>
       </c>
@@ -878,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44222</v>
       </c>
@@ -895,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44223</v>
       </c>
@@ -912,7 +911,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44224</v>
       </c>
@@ -929,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44225</v>
       </c>
@@ -946,7 +945,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44226</v>
       </c>
@@ -963,7 +962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44227</v>
       </c>
@@ -980,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44228</v>
       </c>
@@ -997,7 +996,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>44229</v>
       </c>
@@ -1014,7 +1013,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>44230</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44231</v>
       </c>
@@ -1048,7 +1047,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44232</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44233</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44234</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44235</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44236</v>
       </c>
@@ -1133,7 +1132,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44237</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44238</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44239</v>
       </c>
@@ -1184,7 +1183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44240</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44241</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44242</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44243</v>
       </c>
@@ -1252,7 +1251,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44244</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44245</v>
       </c>
@@ -1286,7 +1285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44246</v>
       </c>
@@ -1303,7 +1302,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44247</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44248</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44249</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44250</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44251</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44252</v>
       </c>
@@ -1405,7 +1404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44253</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44254</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44255</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44256</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44257</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44258</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44259</v>
       </c>
@@ -1524,7 +1523,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44260</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44261</v>
       </c>
@@ -1558,7 +1557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44262</v>
       </c>
@@ -1575,7 +1574,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44263</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>44264</v>
       </c>
@@ -1609,7 +1608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>44265</v>
       </c>
@@ -1626,7 +1625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>44266</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>44267</v>
       </c>
@@ -1660,7 +1659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>44268</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>44269</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>44270</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>44271</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>44272</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>44273</v>
       </c>
@@ -1762,7 +1761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>44274</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>44275</v>
       </c>
@@ -1796,7 +1795,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44276</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44277</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44278</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44279</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44280</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44281</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44282</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44283</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44284</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44285</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44286</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44287</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44288</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44289</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>44290</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>44291</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>44292</v>
       </c>
@@ -2085,7 +2084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>44293</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>44294</v>
       </c>
@@ -2119,7 +2118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>44295</v>
       </c>
@@ -2136,7 +2135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>44296</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>44297</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>44298</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>44299</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>44300</v>
       </c>
@@ -2221,7 +2220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>44301</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>44302</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>44303</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>44304</v>
       </c>
@@ -2289,7 +2288,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>44305</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>44306</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>44307</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>44308</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>44309</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>44310</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>44311</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>44312</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>44313</v>
       </c>
@@ -2442,7 +2441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>44314</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>44315</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>44316</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>44317</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>44318</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>44319</v>
       </c>
@@ -2544,7 +2543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>44320</v>
       </c>
@@ -2561,7 +2560,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>44321</v>
       </c>
@@ -2578,7 +2577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>44322</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>44323</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>44324</v>
       </c>
@@ -2629,7 +2628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>44325</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>44326</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>44327</v>
       </c>
@@ -2680,7 +2679,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>44328</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>44329</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>44330</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>44331</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>44332</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>44333</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>44334</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>44335</v>
       </c>
@@ -2816,7 +2815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>44336</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>44337</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>44338</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>44339</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>44340</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>44341</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>44342</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>44343</v>
       </c>
@@ -2952,7 +2951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>44344</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>44345</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>44346</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>44347</v>
       </c>
@@ -3020,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>44348</v>
       </c>
@@ -3037,7 +3036,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>44349</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>44350</v>
       </c>
@@ -3071,7 +3070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>44351</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>44352</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>44353</v>
       </c>
@@ -3122,7 +3121,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>44354</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>44355</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>44356</v>
       </c>
@@ -3173,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>44357</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>44358</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>44359</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>44360</v>
       </c>
@@ -3241,7 +3240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>44361</v>
       </c>
@@ -3258,7 +3257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>44362</v>
       </c>
@@ -3275,7 +3274,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
         <v>44363</v>
       </c>
@@ -3292,7 +3291,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>44364</v>
       </c>
@@ -3309,7 +3308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>44365</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
         <v>44366</v>
       </c>
@@ -3343,7 +3342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>44367</v>
       </c>
@@ -3360,7 +3359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>44368</v>
       </c>
@@ -3377,7 +3376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>44369</v>
       </c>
@@ -3394,7 +3393,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>44370</v>
       </c>
@@ -3411,7 +3410,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>44371</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>44372</v>
       </c>
@@ -3445,7 +3444,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>44373</v>
       </c>
@@ -3462,7 +3461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>44374</v>
       </c>
@@ -3479,7 +3478,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>44375</v>
       </c>
@@ -3496,7 +3495,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>44376</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>44377</v>
       </c>
@@ -3530,7 +3529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>44378</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>44379</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>44380</v>
       </c>
@@ -3581,7 +3580,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>44381</v>
       </c>
@@ -3598,7 +3597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>44382</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>44383</v>
       </c>
@@ -3632,7 +3631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>44384</v>
       </c>
@@ -3649,7 +3648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>44385</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>44386</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>44387</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>44388</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>44389</v>
       </c>
@@ -3734,7 +3733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
         <v>44390</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>44391</v>
       </c>
@@ -3768,7 +3767,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
         <v>44392</v>
       </c>
@@ -3785,7 +3784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>44393</v>
       </c>
@@ -3802,7 +3801,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
         <v>44394</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>44395</v>
       </c>
@@ -3836,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
         <v>44396</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
         <v>44397</v>
       </c>
@@ -3870,7 +3869,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
         <v>44398</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
         <v>44399</v>
       </c>
@@ -3904,7 +3903,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>44400</v>
       </c>
@@ -3921,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
         <v>44401</v>
       </c>
@@ -3938,7 +3937,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
         <v>44402</v>
       </c>
@@ -3955,7 +3954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
         <v>44403</v>
       </c>
@@ -3972,7 +3971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
         <v>44404</v>
       </c>
@@ -3989,7 +3988,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
         <v>44405</v>
       </c>
@@ -4006,7 +4005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
         <v>44406</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
         <v>44407</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
         <v>44408</v>
       </c>
@@ -4057,7 +4056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
         <v>44409</v>
       </c>
@@ -4074,7 +4073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
         <v>44410</v>
       </c>
@@ -4091,7 +4090,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
         <v>44411</v>
       </c>
@@ -4108,7 +4107,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
         <v>44412</v>
       </c>
@@ -4125,7 +4124,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
         <v>44413</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
         <v>44414</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
         <v>44415</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
         <v>44416</v>
       </c>
@@ -4193,7 +4192,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
         <v>44417</v>
       </c>
@@ -4210,7 +4209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
         <v>44418</v>
       </c>
@@ -4227,7 +4226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
         <v>44419</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
         <v>44420</v>
       </c>
@@ -4261,7 +4260,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
         <v>44421</v>
       </c>
@@ -4278,7 +4277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
         <v>44422</v>
       </c>
@@ -4295,7 +4294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
         <v>44423</v>
       </c>
@@ -4312,7 +4311,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
         <v>44424</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
         <v>44425</v>
       </c>
@@ -4346,7 +4345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
         <v>44426</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
         <v>44427</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
         <v>44428</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
         <v>44429</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
         <v>44430</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
         <v>44431</v>
       </c>
@@ -4448,7 +4447,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
         <v>44432</v>
       </c>
@@ -4465,7 +4464,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
         <v>44433</v>
       </c>
@@ -4482,7 +4481,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
         <v>44434</v>
       </c>
@@ -4499,7 +4498,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
         <v>44435</v>
       </c>
@@ -4516,7 +4515,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
         <v>44436</v>
       </c>
@@ -4533,7 +4532,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
         <v>44437</v>
       </c>
@@ -4550,7 +4549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
         <v>44438</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
         <v>44439</v>
       </c>
@@ -4584,7 +4583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
         <v>44440</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
         <v>44441</v>
       </c>
@@ -4618,7 +4617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
         <v>44442</v>
       </c>
@@ -4635,7 +4634,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
         <v>44443</v>
       </c>
@@ -4652,7 +4651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
         <v>44444</v>
       </c>
@@ -4669,7 +4668,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
         <v>44445</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
         <v>44446</v>
       </c>
@@ -4703,7 +4702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
         <v>44447</v>
       </c>
@@ -4720,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
         <v>44448</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
         <v>44449</v>
       </c>
@@ -4754,7 +4753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
         <v>44450</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
         <v>44451</v>
       </c>
@@ -4788,7 +4787,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
         <v>44452</v>
       </c>
@@ -4805,7 +4804,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
         <v>44453</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
         <v>44454</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
         <v>44455</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
         <v>44456</v>
       </c>
@@ -4873,7 +4872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
         <v>44457</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
         <v>44458</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
         <v>44459</v>
       </c>
@@ -4924,7 +4923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="2">
         <v>44460</v>
       </c>
@@ -4941,7 +4940,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
         <v>44461</v>
       </c>
@@ -4958,7 +4957,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
         <v>44462</v>
       </c>
@@ -4975,7 +4974,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
         <v>44463</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="2">
         <v>44464</v>
       </c>
@@ -5009,7 +5008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
         <v>44465</v>
       </c>
@@ -5026,7 +5025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" s="2">
         <v>44466</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" s="2">
         <v>44467</v>
       </c>
@@ -5060,7 +5059,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" s="2">
         <v>44468</v>
       </c>
@@ -5077,7 +5076,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="2">
         <v>44469</v>
       </c>
@@ -5094,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" s="2">
         <v>44470</v>
       </c>
@@ -5111,7 +5110,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="2">
         <v>44471</v>
       </c>
@@ -5128,7 +5127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="2">
         <v>44472</v>
       </c>
@@ -5145,7 +5144,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" s="2">
         <v>44473</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" s="2">
         <v>44474</v>
       </c>
@@ -5179,7 +5178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="2">
         <v>44475</v>
       </c>
@@ -5196,7 +5195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="2">
         <v>44476</v>
       </c>
@@ -5213,7 +5212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="2">
         <v>44477</v>
       </c>
@@ -5230,7 +5229,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" s="2">
         <v>44478</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" s="2">
         <v>44479</v>
       </c>
@@ -5264,7 +5263,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="2">
         <v>44480</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" s="2">
         <v>44481</v>
       </c>
@@ -5298,7 +5297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" s="2">
         <v>44482</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" s="2">
         <v>44483</v>
       </c>
@@ -5332,7 +5331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" s="2">
         <v>44484</v>
       </c>
@@ -5349,7 +5348,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" s="2">
         <v>44485</v>
       </c>
@@ -5366,7 +5365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" s="2">
         <v>44486</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" s="2">
         <v>44487</v>
       </c>
@@ -5400,7 +5399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" s="2">
         <v>44488</v>
       </c>
@@ -5417,7 +5416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" s="2">
         <v>44489</v>
       </c>
@@ -5434,7 +5433,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" s="2">
         <v>44490</v>
       </c>
@@ -5451,7 +5450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" s="2">
         <v>44491</v>
       </c>
@@ -5468,7 +5467,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" s="2">
         <v>44492</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" s="2">
         <v>44493</v>
       </c>
@@ -5502,7 +5501,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" s="2">
         <v>44494</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A300" s="2">
         <v>44495</v>
       </c>
@@ -5536,7 +5535,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A301" s="2">
         <v>44496</v>
       </c>
@@ -5553,7 +5552,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A302" s="2">
         <v>44497</v>
       </c>
@@ -5570,7 +5569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" s="2">
         <v>44498</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A304" s="2">
         <v>44499</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" s="2">
         <v>44500</v>
       </c>
@@ -5621,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" s="2">
         <v>44501</v>
       </c>
@@ -5638,7 +5637,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" s="2">
         <v>44502</v>
       </c>
@@ -5655,7 +5654,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" s="2">
         <v>44503</v>
       </c>
@@ -5672,7 +5671,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" s="2">
         <v>44504</v>
       </c>
@@ -5689,7 +5688,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" s="2">
         <v>44505</v>
       </c>
@@ -5706,7 +5705,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" s="2">
         <v>44506</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A312" s="2">
         <v>44507</v>
       </c>
@@ -5740,7 +5739,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" s="2">
         <v>44508</v>
       </c>
@@ -5757,7 +5756,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" s="2">
         <v>44509</v>
       </c>
@@ -5774,7 +5773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" s="2">
         <v>44510</v>
       </c>
@@ -5791,7 +5790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" s="2">
         <v>44511</v>
       </c>
@@ -5808,7 +5807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" s="2">
         <v>44512</v>
       </c>
@@ -5825,7 +5824,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" s="2">
         <v>44513</v>
       </c>
@@ -5842,7 +5841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="2">
         <v>44514</v>
       </c>
@@ -5859,7 +5858,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" s="2">
         <v>44515</v>
       </c>
@@ -5876,7 +5875,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" s="2">
         <v>44516</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" s="2">
         <v>44517</v>
       </c>
@@ -5910,7 +5909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" s="2">
         <v>44518</v>
       </c>
@@ -5927,7 +5926,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" s="2">
         <v>44519</v>
       </c>
@@ -5944,7 +5943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" s="2">
         <v>44520</v>
       </c>
@@ -5961,7 +5960,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" s="2">
         <v>44521</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" s="2">
         <v>44522</v>
       </c>
@@ -5995,7 +5994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" s="2">
         <v>44523</v>
       </c>
@@ -6012,7 +6011,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" s="2">
         <v>44524</v>
       </c>
@@ -6029,7 +6028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" s="2">
         <v>44525</v>
       </c>
@@ -6046,7 +6045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A331" s="2">
         <v>44526</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A332" s="2">
         <v>44527</v>
       </c>
@@ -6080,7 +6079,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A333" s="2">
         <v>44528</v>
       </c>
@@ -6097,7 +6096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A334" s="2">
         <v>44529</v>
       </c>
@@ -6114,7 +6113,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A335" s="2">
         <v>44530</v>
       </c>
@@ -6131,7 +6130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A336" s="2">
         <v>44531</v>
       </c>
@@ -6148,7 +6147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" s="2">
         <v>44532</v>
       </c>
@@ -6165,7 +6164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" s="2">
         <v>44533</v>
       </c>
@@ -6182,7 +6181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" s="2">
         <v>44534</v>
       </c>
@@ -6199,7 +6198,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" s="2">
         <v>44535</v>
       </c>
@@ -6216,7 +6215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" s="2">
         <v>44536</v>
       </c>
@@ -6233,7 +6232,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A342" s="2">
         <v>44537</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="343" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A343" s="2">
         <v>44538</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" s="2">
         <v>44539</v>
       </c>
@@ -6284,7 +6283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" s="2">
         <v>44540</v>
       </c>
@@ -6301,7 +6300,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" s="2">
         <v>44541</v>
       </c>
@@ -6318,7 +6317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" s="2">
         <v>44542</v>
       </c>
@@ -6335,7 +6334,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" s="2">
         <v>44543</v>
       </c>
@@ -6352,7 +6351,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" s="2">
         <v>44544</v>
       </c>
@@ -6369,7 +6368,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" s="2">
         <v>44545</v>
       </c>
@@ -6386,7 +6385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" s="2">
         <v>44546</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" s="2">
         <v>44547</v>
       </c>
@@ -6420,7 +6419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" s="2">
         <v>44548</v>
       </c>
@@ -6437,7 +6436,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" s="2">
         <v>44549</v>
       </c>
@@ -6454,7 +6453,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="355" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A355" s="2">
         <v>44550</v>
       </c>
@@ -6471,7 +6470,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" s="2">
         <v>44551</v>
       </c>
@@ -6488,7 +6487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A357" s="2">
         <v>44552</v>
       </c>
@@ -6505,7 +6504,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="358" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" s="2">
         <v>44553</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="359" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" s="2">
         <v>44554</v>
       </c>
@@ -6539,7 +6538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="360" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A360" s="2">
         <v>44555</v>
       </c>
@@ -6556,7 +6555,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="361" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A361" s="2">
         <v>44556</v>
       </c>
@@ -6573,7 +6572,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="362" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" s="2">
         <v>44557</v>
       </c>
@@ -6590,7 +6589,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="363" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" s="2">
         <v>44558</v>
       </c>
@@ -6607,7 +6606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="364" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" s="2">
         <v>44559</v>
       </c>
@@ -6624,7 +6623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="365" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A365" s="2">
         <v>44560</v>
       </c>
@@ -6641,7 +6640,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="366" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A366" s="2">
         <v>44561</v>
       </c>
@@ -6658,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A367" s="2">
         <v>44562</v>
       </c>
@@ -6675,7 +6674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A368" s="2">
         <v>44563</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="369" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A369" s="2">
         <v>44564</v>
       </c>
@@ -6709,7 +6708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="370" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A370" s="2">
         <v>44565</v>
       </c>
@@ -6726,7 +6725,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="371" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A371" s="2">
         <v>44566</v>
       </c>
@@ -6743,7 +6742,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="372" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A372" s="2">
         <v>44567</v>
       </c>
@@ -6760,7 +6759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="373" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A373" s="2">
         <v>44568</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="374" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A374" s="2">
         <v>44569</v>
       </c>
@@ -6794,7 +6793,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="375" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A375" s="2">
         <v>44570</v>
       </c>
@@ -6811,7 +6810,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="376" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A376" s="2">
         <v>44571</v>
       </c>
@@ -6828,7 +6827,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="377" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A377" s="2">
         <v>44572</v>
       </c>
@@ -6845,7 +6844,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="378" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A378" s="2">
         <v>44573</v>
       </c>
@@ -6862,7 +6861,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="379" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A379" s="2">
         <v>44574</v>
       </c>
@@ -6879,7 +6878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="380" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A380" s="2">
         <v>44575</v>
       </c>
@@ -6896,7 +6895,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="381" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A381" s="2">
         <v>44576</v>
       </c>
@@ -6913,7 +6912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="382" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A382" s="2">
         <v>44577</v>
       </c>
@@ -6930,7 +6929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A383" s="2">
         <v>44578</v>
       </c>
@@ -6947,7 +6946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A384" s="2">
         <v>44579</v>
       </c>
@@ -6964,7 +6963,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="385" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A385" s="2">
         <v>44580</v>
       </c>
@@ -6981,7 +6980,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="386" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A386" s="2">
         <v>44581</v>
       </c>
@@ -6998,7 +6997,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="387" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A387" s="2">
         <v>44582</v>
       </c>
@@ -7015,7 +7014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="388" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A388" s="2">
         <v>44583</v>
       </c>
@@ -7032,7 +7031,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="389" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A389" s="2">
         <v>44584</v>
       </c>
@@ -7049,7 +7048,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="390" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A390" s="2">
         <v>44585</v>
       </c>
@@ -7066,7 +7065,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="391" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A391" s="2">
         <v>44586</v>
       </c>
@@ -7083,7 +7082,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="392" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A392" s="2">
         <v>44587</v>
       </c>
@@ -7100,7 +7099,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="393" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A393" s="2">
         <v>44588</v>
       </c>
@@ -7117,7 +7116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="394" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A394" s="2">
         <v>44589</v>
       </c>
@@ -7134,7 +7133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="395" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A395" s="2">
         <v>44590</v>
       </c>
@@ -7151,7 +7150,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="396" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A396" s="2">
         <v>44591</v>
       </c>
@@ -7168,7 +7167,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="397" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A397" s="2">
         <v>44592</v>
       </c>
@@ -7185,7 +7184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A398" s="2">
         <v>44593</v>
       </c>
@@ -7202,7 +7201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="399" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A399" s="2">
         <v>44594</v>
       </c>
@@ -7219,7 +7218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="400" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A400" s="2">
         <v>44595</v>
       </c>
@@ -7236,7 +7235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A401" s="2">
         <v>44596</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A402" s="2">
         <v>44597</v>
       </c>
@@ -7270,7 +7269,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A403" s="2">
         <v>44598</v>
       </c>
@@ -7287,7 +7286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A404" s="2">
         <v>44599</v>
       </c>
@@ -7304,7 +7303,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A405" s="2">
         <v>44600</v>
       </c>
@@ -7321,7 +7320,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A406" s="2">
         <v>44601</v>
       </c>
@@ -7338,7 +7337,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A407" s="2">
         <v>44602</v>
       </c>
@@ -7355,7 +7354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A408" s="2">
         <v>44603</v>
       </c>
@@ -7372,7 +7371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A409" s="2">
         <v>44604</v>
       </c>
@@ -7389,7 +7388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A410" s="2">
         <v>44605</v>
       </c>
@@ -7406,7 +7405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A411" s="2">
         <v>44606</v>
       </c>
@@ -7423,7 +7422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A412" s="2">
         <v>44607</v>
       </c>
@@ -7440,7 +7439,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="413" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A413" s="2">
         <v>44608</v>
       </c>
@@ -7457,7 +7456,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A414" s="2">
         <v>44609</v>
       </c>
@@ -7474,7 +7473,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A415" s="2">
         <v>44610</v>
       </c>
@@ -7491,7 +7490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A416" s="2">
         <v>44611</v>
       </c>
@@ -7508,7 +7507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A417" s="2">
         <v>44612</v>
       </c>
@@ -7525,7 +7524,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A418" s="2">
         <v>44613</v>
       </c>
@@ -7542,7 +7541,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A419" s="2">
         <v>44614</v>
       </c>
@@ -7559,7 +7558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="420" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A420" s="2">
         <v>44615</v>
       </c>
@@ -7576,7 +7575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A421" s="2">
         <v>44616</v>
       </c>
@@ -7593,7 +7592,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A422" s="2">
         <v>44617</v>
       </c>
@@ -7610,7 +7609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A423" s="2">
         <v>44618</v>
       </c>
@@ -7627,7 +7626,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A424" s="2">
         <v>44619</v>
       </c>
@@ -7644,7 +7643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A425" s="2">
         <v>44620</v>
       </c>
@@ -7661,7 +7660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A426" s="2">
         <v>44621</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A427" s="2">
         <v>44622</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A428" s="2">
         <v>44623</v>
       </c>
@@ -7712,7 +7711,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A429" s="2">
         <v>44624</v>
       </c>
@@ -7729,7 +7728,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A430" s="2">
         <v>44625</v>
       </c>
@@ -7746,7 +7745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A431" s="2">
         <v>44626</v>
       </c>
@@ -7763,7 +7762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A432" s="2">
         <v>44627</v>
       </c>
@@ -7780,7 +7779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="433" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A433" s="2">
         <v>44628</v>
       </c>
@@ -7797,7 +7796,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="434" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A434" s="2">
         <v>44629</v>
       </c>
@@ -7814,7 +7813,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="435" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A435" s="2">
         <v>44630</v>
       </c>
@@ -7831,7 +7830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="436" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A436" s="2">
         <v>44631</v>
       </c>
@@ -7848,7 +7847,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="437" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A437" s="2">
         <v>44632</v>
       </c>
@@ -7865,7 +7864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="438" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A438" s="2">
         <v>44633</v>
       </c>
@@ -7882,7 +7881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="439" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A439" s="2">
         <v>44634</v>
       </c>
@@ -7899,7 +7898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A440" s="2">
         <v>44635</v>
       </c>
@@ -7916,7 +7915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="441" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A441" s="2">
         <v>44636</v>
       </c>
@@ -7933,7 +7932,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="442" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A442" s="2">
         <v>44637</v>
       </c>
@@ -7950,7 +7949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="443" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A443" s="2">
         <v>44638</v>
       </c>
@@ -7967,7 +7966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="444" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A444" s="2">
         <v>44639</v>
       </c>
@@ -7984,7 +7983,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="445" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A445" s="2">
         <v>44640</v>
       </c>
@@ -8001,7 +8000,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="446" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A446" s="2">
         <v>44641</v>
       </c>
@@ -8018,7 +8017,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="447" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A447" s="2">
         <v>44642</v>
       </c>
@@ -8035,7 +8034,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="448" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A448" s="2">
         <v>44643</v>
       </c>
@@ -8052,7 +8051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="449" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A449" s="2">
         <v>44644</v>
       </c>
@@ -8069,7 +8068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="450" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A450" s="2">
         <v>44645</v>
       </c>
@@ -8086,7 +8085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="451" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A451" s="2">
         <v>44646</v>
       </c>
@@ -8103,7 +8102,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="452" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A452" s="2">
         <v>44647</v>
       </c>
@@ -8120,7 +8119,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="453" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A453" s="2">
         <v>44648</v>
       </c>
@@ -8137,7 +8136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="454" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A454" s="2">
         <v>44649</v>
       </c>
@@ -8171,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A456" s="2">
         <v>44651</v>
       </c>
@@ -8188,7 +8187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="457" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A457" s="2">
         <v>44652</v>
       </c>
@@ -8205,7 +8204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="458" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A458" s="2">
         <v>44653</v>
       </c>
@@ -8222,7 +8221,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="459" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A459" s="2">
         <v>44654</v>
       </c>
@@ -8239,7 +8238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="460" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A460" s="2">
         <v>44655</v>
       </c>
@@ -8256,7 +8255,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="461" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A461" s="2">
         <v>44656</v>
       </c>
@@ -8273,7 +8272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="462" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A462" s="2">
         <v>44657</v>
       </c>
@@ -8290,7 +8289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="463" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A463" s="2">
         <v>44658</v>
       </c>
@@ -8307,7 +8306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="464" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A464" s="2">
         <v>44659</v>
       </c>
@@ -8324,7 +8323,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="465" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A465" s="2">
         <v>44660</v>
       </c>
@@ -8341,7 +8340,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="466" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A466" s="2">
         <v>44661</v>
       </c>
@@ -8358,7 +8357,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="467" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A467" s="2">
         <v>44662</v>
       </c>
@@ -8375,7 +8374,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="468" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A468" s="2">
         <v>44663</v>
       </c>
@@ -8392,7 +8391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="469" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A469" s="2">
         <v>44664</v>
       </c>
@@ -8409,7 +8408,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="470" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A470" s="2">
         <v>44665</v>
       </c>
@@ -8426,7 +8425,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="471" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A471" s="2">
         <v>44666</v>
       </c>
@@ -8443,7 +8442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="472" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A472" s="2">
         <v>44667</v>
       </c>
@@ -8460,7 +8459,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="473" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A473" s="2">
         <v>44668</v>
       </c>
@@ -8477,7 +8476,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="474" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A474" s="2">
         <v>44669</v>
       </c>
@@ -8494,7 +8493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="475" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A475" s="2">
         <v>44670</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="476" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A476" s="2">
         <v>44671</v>
       </c>
@@ -8528,7 +8527,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="477" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A477" s="2">
         <v>44672</v>
       </c>
@@ -8545,7 +8544,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="478" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A478" s="2">
         <v>44673</v>
       </c>
@@ -8562,7 +8561,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="479" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A479" s="2">
         <v>44674</v>
       </c>
@@ -8579,7 +8578,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="480" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A480" s="2">
         <v>44675</v>
       </c>
@@ -8596,7 +8595,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="481" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A481" s="2">
         <v>44676</v>
       </c>
@@ -8613,7 +8612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="482" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A482" s="2">
         <v>44677</v>
       </c>
@@ -8630,7 +8629,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="483" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A483" s="2">
         <v>44678</v>
       </c>
@@ -8647,7 +8646,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="484" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A484" s="2">
         <v>44679</v>
       </c>
@@ -8664,7 +8663,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="485" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A485" s="2">
         <v>44680</v>
       </c>
@@ -8681,7 +8680,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="486" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A486" s="2">
         <v>44681</v>
       </c>
@@ -8698,7 +8697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="487" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A487" s="2">
         <v>44682</v>
       </c>
@@ -8715,7 +8714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="488" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A488" s="2">
         <v>44683</v>
       </c>
@@ -8732,7 +8731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="489" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A489" s="2">
         <v>44684</v>
       </c>
@@ -8749,7 +8748,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="490" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A490" s="2">
         <v>44685</v>
       </c>
@@ -8766,7 +8765,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="491" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A491" s="2">
         <v>44686</v>
       </c>
@@ -8783,7 +8782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="492" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A492" s="2">
         <v>44687</v>
       </c>
@@ -8800,7 +8799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="493" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A493" s="2">
         <v>44688</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="494" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A494" s="2">
         <v>44689</v>
       </c>
@@ -8834,7 +8833,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="495" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A495" s="2">
         <v>44690</v>
       </c>
@@ -8851,7 +8850,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="496" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A496" s="2">
         <v>44691</v>
       </c>
@@ -8868,7 +8867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="497" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A497" s="2">
         <v>44692</v>
       </c>
@@ -8885,7 +8884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="498" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A498" s="2">
         <v>44693</v>
       </c>
@@ -8902,7 +8901,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="499" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A499" s="2">
         <v>44694</v>
       </c>
@@ -8920,16 +8919,40 @@
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A500" s="2"/>
+      <c r="A500" s="2">
+        <v>44695</v>
+      </c>
+      <c r="B500" s="1">
+        <v>98</v>
+      </c>
+      <c r="C500" s="1">
+        <v>50</v>
+      </c>
+      <c r="D500" s="1">
+        <v>19</v>
+      </c>
+      <c r="E500" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A501" s="2">
+        <v>44696</v>
+      </c>
+      <c r="B501" s="1">
+        <v>3</v>
+      </c>
+      <c r="C501" s="1">
+        <v>0</v>
+      </c>
+      <c r="D501" s="1">
+        <v>66</v>
+      </c>
+      <c r="E501" s="1">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E499" xr:uid="{4F7DFC0D-7099-4BD6-B583-485D9FE3FFF5}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="--"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>